<commit_message>
small fix method find_max2
</commit_message>
<xml_diff>
--- a/analiserResults_inputMinS3Int.xlsx
+++ b/analiserResults_inputMinS3Int.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alduck/Documents/GitHub/SelectingMRs_FuzzerBasedApproach/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0FE7AE-B0E6-9F46-8077-471318869ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EAC4DF-A42C-C04B-AC45-0AD85F165ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - analiserResults_input" sheetId="1" r:id="rId1"/>
@@ -225,17 +225,20 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -909,23 +912,23 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1054,7 +1057,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-            <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+            <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -2202,7 +2205,7 @@
   <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="X35" sqref="X35"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2232,28 +2235,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
+      <c r="A1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
     </row>
     <row r="2" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -2978,23 +2981,23 @@
       <c r="N13" s="24">
         <v>0</v>
       </c>
-      <c r="O13" s="35">
-        <v>1</v>
-      </c>
-      <c r="P13" s="33">
-        <v>74</v>
-      </c>
-      <c r="Q13" s="34">
-        <v>26</v>
-      </c>
-      <c r="R13" s="35">
-        <v>1</v>
-      </c>
-      <c r="S13" s="33">
-        <v>87</v>
-      </c>
-      <c r="T13" s="34">
-        <v>13</v>
+      <c r="O13" s="26">
+        <v>1</v>
+      </c>
+      <c r="P13" s="23">
+        <v>100</v>
+      </c>
+      <c r="Q13" s="24">
+        <v>0</v>
+      </c>
+      <c r="R13" s="26">
+        <v>1</v>
+      </c>
+      <c r="S13" s="23">
+        <v>100</v>
+      </c>
+      <c r="T13" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="22" customHeight="1" x14ac:dyDescent="0.15">
@@ -3866,126 +3869,131 @@
       </c>
     </row>
     <row r="30" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="57" t="s">
+      <c r="C30" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="57" t="s">
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="57"/>
     </row>
     <row r="31" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56" t="s">
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
     </row>
     <row r="32" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="55" t="s">
+      <c r="B32" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="56" t="s">
+      <c r="C32" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56" t="s">
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="55"/>
     </row>
     <row r="33" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="55" t="s">
+      <c r="B33" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="56" t="s">
+      <c r="C33" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56" t="s">
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="55"/>
     </row>
     <row r="34" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="56" t="s">
+      <c r="C34" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56" t="s">
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="55"/>
     </row>
     <row r="35" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="55" t="s">
+      <c r="B35" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56" t="s">
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="55"/>
+      <c r="J35" s="55"/>
     </row>
     <row r="36" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="55" t="s">
+      <c r="B36" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56" t="s">
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="H36" s="56"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="56"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C33:F33"/>
     <mergeCell ref="G36:J36"/>
     <mergeCell ref="C36:F36"/>
     <mergeCell ref="C34:F34"/>
@@ -3996,11 +4004,6 @@
     <mergeCell ref="G33:J33"/>
     <mergeCell ref="G34:J34"/>
     <mergeCell ref="G35:J35"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="52" orientation="landscape"/>

</xml_diff>